<commit_message>
update bbg data to 6/30/2023
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_data/ups_data.xlsx
+++ b/EquityHedging/data/update_data/ups_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pforj\Documents\ups\RMP\EquityHedging\data\update_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95F4A0F-D29F-4FC3-A01C-9EF6528297FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B4880B-8350-409E-97A0-46AFD7A9947D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="5490" windowWidth="28110" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8985" yWindow="1980" windowWidth="28110" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
@@ -164,87 +164,49 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|12809649761530360839</stp>
-        <tr r="N7" s="4"/>
+        <stp>BDH|18290936258475145947</stp>
+        <tr r="E7" s="4"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|15483021618866917972</stp>
-        <tr r="G7" s="4"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|10670352342178774678</stp>
-        <tr r="R7" s="4"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|10896894843648603839</stp>
-        <tr r="P7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17050122050196743936</stp>
-        <tr r="D7" s="4"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|13392134017130383301</stp>
-        <tr r="F7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|16143997285944048338</stp>
-        <tr r="Q7" s="4"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|10699851695189017946</stp>
-        <tr r="L7" s="4"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17393619555144492435</stp>
-        <tr r="C7" s="4"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|5201333315403192945</stp>
-        <tr r="H7" s="4"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|5794910272568063748</stp>
+        <stp>BDH|11863209313204424822</stp>
         <tr r="J7" s="4"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|5760436651721918198</stp>
+        <stp>BDH|12553163983537424383</stp>
+        <tr r="H7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|15687205993343727151</stp>
+        <tr r="O7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|12109213214685379461</stp>
+        <tr r="Q7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|12229018108914937742</stp>
+        <tr r="M7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17398358938439631887</stp>
+        <tr r="I7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|15760512430632677745</stp>
         <tr r="A7" s="4"/>
       </tp>
     </main>
@@ -252,32 +214,56 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|4966307451894559072</stp>
-        <tr r="O7" s="4"/>
+        <stp>BDH|4331629719708859364</stp>
+        <tr r="D7" s="4"/>
       </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|4053006154030137697</stp>
-        <tr r="K7" s="4"/>
+        <stp>BDH|4529507267297535465</stp>
+        <tr r="N7" s="4"/>
       </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|5673633219301958358</stp>
-        <tr r="M7" s="4"/>
+        <stp>BDH|7158556662108784907</stp>
+        <tr r="R7" s="4"/>
       </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|2386374816867304629</stp>
-        <tr r="E7" s="4"/>
+        <stp>BDH|2464811926455430816</stp>
+        <tr r="C7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|1070361247123342311</stp>
+        <tr r="G7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|5906030544325357432</stp>
+        <tr r="L7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|7411529915306178520</stp>
+        <tr r="F7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|1878665362808563879</stp>
+        <tr r="P7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|7649255472192013379</stp>
+        <tr r="K7" s="4"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -416,14 +402,6 @@
         <stp>[ups_data.xlsx]bbg!R5C4</stp>
         <stp>PX_LAST</stp>
         <tr r="D5" s="4"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|823905859281847538</stp>
-        <tr r="I7" s="4"/>
       </tp>
     </main>
   </volType>
@@ -693,7 +671,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R332"/>
+  <dimension ref="A1:R397"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -732,7 +710,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="1">
-        <v>45016</v>
+        <v>45107</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -916,74 +894,74 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=326")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S","cols=2;rows=391")</f>
         <v>44561</v>
       </c>
       <c r="B7">
         <v>9986.6980000000003</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>9491.1</v>
       </c>
       <c r="D7">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>389.04</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>5233.6899999999996</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>214.08</v>
       </c>
       <c r="G7">
-        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>122.8967</v>
       </c>
       <c r="H7">
-        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>175.14</v>
       </c>
       <c r="I7">
-        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>98.672499999999999</v>
       </c>
       <c r="J7">
-        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>101.2684</v>
       </c>
       <c r="K7">
-        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>135.21369999999999</v>
       </c>
       <c r="L7">
-        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>835.24</v>
       </c>
       <c r="M7">
-        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>1088</v>
       </c>
       <c r="N7">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>297.6395</v>
       </c>
       <c r="O7">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>287.23</v>
       </c>
       <c r="P7">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>368.34</v>
       </c>
       <c r="Q7">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>345.76</v>
       </c>
       <c r="R7">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=326")</f>
+        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H","cols=1;rows=391")</f>
         <v>169.35</v>
       </c>
     </row>
@@ -19185,6 +19163,3646 @@
       </c>
       <c r="R332">
         <v>165.93</v>
+      </c>
+    </row>
+    <row r="333" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A333" s="1">
+        <v>45019</v>
+      </c>
+      <c r="B333">
+        <v>8823.6550000000007</v>
+      </c>
+      <c r="C333">
+        <v>9802.48</v>
+      </c>
+      <c r="D333">
+        <v>342.11</v>
+      </c>
+      <c r="E333">
+        <v>4128.05</v>
+      </c>
+      <c r="F333">
+        <v>144.77000000000001</v>
+      </c>
+      <c r="G333">
+        <v>104.0163</v>
+      </c>
+      <c r="H333">
+        <v>163.63999999999999</v>
+      </c>
+      <c r="I333">
+        <v>86.340500000000006</v>
+      </c>
+      <c r="J333">
+        <v>88.0989</v>
+      </c>
+      <c r="K333">
+        <v>123.2276</v>
+      </c>
+      <c r="L333">
+        <v>878.5</v>
+      </c>
+      <c r="M333">
+        <v>1116.1199999999999</v>
+      </c>
+      <c r="N333">
+        <v>275.45209999999997</v>
+      </c>
+      <c r="O333">
+        <v>278.62</v>
+      </c>
+      <c r="P333">
+        <v>351.72</v>
+      </c>
+      <c r="Q333">
+        <v>330.94</v>
+      </c>
+      <c r="R333">
+        <v>166.3</v>
+      </c>
+    </row>
+    <row r="334" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A334" s="1">
+        <v>45020</v>
+      </c>
+      <c r="B334">
+        <v>8773.3080000000009</v>
+      </c>
+      <c r="C334">
+        <v>9812.19</v>
+      </c>
+      <c r="D334">
+        <v>341.33</v>
+      </c>
+      <c r="E334">
+        <v>4140.5600000000004</v>
+      </c>
+      <c r="F334">
+        <v>145.72999999999999</v>
+      </c>
+      <c r="G334">
+        <v>104.05719999999999</v>
+      </c>
+      <c r="H334">
+        <v>163.63999999999999</v>
+      </c>
+      <c r="I334">
+        <v>86.361599999999996</v>
+      </c>
+      <c r="J334">
+        <v>88.096400000000003</v>
+      </c>
+      <c r="K334">
+        <v>123.235</v>
+      </c>
+      <c r="L334">
+        <v>879.51</v>
+      </c>
+      <c r="M334">
+        <v>1116.97</v>
+      </c>
+      <c r="N334">
+        <v>275.63040000000001</v>
+      </c>
+      <c r="O334">
+        <v>278.73</v>
+      </c>
+      <c r="P334">
+        <v>351.77</v>
+      </c>
+      <c r="Q334">
+        <v>331.01</v>
+      </c>
+      <c r="R334">
+        <v>166.48</v>
+      </c>
+    </row>
+    <row r="335" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A335" s="1">
+        <v>45021</v>
+      </c>
+      <c r="B335">
+        <v>8752.5429999999997</v>
+      </c>
+      <c r="C335">
+        <v>9773.6200000000008</v>
+      </c>
+      <c r="D335">
+        <v>339.99</v>
+      </c>
+      <c r="E335">
+        <v>4161.84</v>
+      </c>
+      <c r="F335">
+        <v>147.54</v>
+      </c>
+      <c r="G335">
+        <v>104.0401</v>
+      </c>
+      <c r="H335">
+        <v>163.56</v>
+      </c>
+      <c r="I335">
+        <v>86.356099999999998</v>
+      </c>
+      <c r="J335">
+        <v>88.103499999999997</v>
+      </c>
+      <c r="K335">
+        <v>123.2296</v>
+      </c>
+      <c r="L335">
+        <v>880.23</v>
+      </c>
+      <c r="M335">
+        <v>1119.04</v>
+      </c>
+      <c r="N335">
+        <v>275.66059999999999</v>
+      </c>
+      <c r="O335">
+        <v>279.01</v>
+      </c>
+      <c r="P335">
+        <v>352.1</v>
+      </c>
+      <c r="Q335">
+        <v>331.11</v>
+      </c>
+      <c r="R335">
+        <v>166.76</v>
+      </c>
+    </row>
+    <row r="336" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A336" s="1">
+        <v>45022</v>
+      </c>
+      <c r="B336">
+        <v>8785.7019999999993</v>
+      </c>
+      <c r="C336">
+        <v>9806.59</v>
+      </c>
+      <c r="D336">
+        <v>340.58</v>
+      </c>
+      <c r="E336">
+        <v>4167.8500000000004</v>
+      </c>
+      <c r="F336">
+        <v>148.13</v>
+      </c>
+      <c r="G336">
+        <v>103.93040000000001</v>
+      </c>
+      <c r="H336">
+        <v>163.62</v>
+      </c>
+      <c r="I336">
+        <v>86.314099999999996</v>
+      </c>
+      <c r="J336">
+        <v>88.0732</v>
+      </c>
+      <c r="K336">
+        <v>123.2101</v>
+      </c>
+      <c r="L336">
+        <v>879.7</v>
+      </c>
+      <c r="M336">
+        <v>1119.3399999999999</v>
+      </c>
+      <c r="N336">
+        <v>275.6943</v>
+      </c>
+      <c r="O336">
+        <v>279.13</v>
+      </c>
+      <c r="P336">
+        <v>352.52</v>
+      </c>
+      <c r="Q336">
+        <v>331.57</v>
+      </c>
+      <c r="R336">
+        <v>166.86</v>
+      </c>
+    </row>
+    <row r="337" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A337" s="1">
+        <v>45023</v>
+      </c>
+      <c r="B337">
+        <v>8785.7019999999993</v>
+      </c>
+      <c r="C337">
+        <v>9806.59</v>
+      </c>
+      <c r="D337">
+        <v>340.71</v>
+      </c>
+      <c r="E337">
+        <v>4128.95</v>
+      </c>
+      <c r="F337">
+        <v>146.21</v>
+      </c>
+      <c r="G337">
+        <v>103.93040000000001</v>
+      </c>
+      <c r="H337">
+        <v>163.62</v>
+      </c>
+      <c r="I337">
+        <v>86.314099999999996</v>
+      </c>
+      <c r="J337">
+        <v>88.0732</v>
+      </c>
+      <c r="K337">
+        <v>123.2101</v>
+      </c>
+      <c r="L337">
+        <v>879.7</v>
+      </c>
+      <c r="M337">
+        <v>1119.3399999999999</v>
+      </c>
+      <c r="N337">
+        <v>275.6943</v>
+      </c>
+      <c r="O337">
+        <v>279.13</v>
+      </c>
+      <c r="P337">
+        <v>352.52</v>
+      </c>
+      <c r="Q337">
+        <v>331.57</v>
+      </c>
+      <c r="R337">
+        <v>166.86</v>
+      </c>
+    </row>
+    <row r="338" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A338" s="1">
+        <v>45026</v>
+      </c>
+      <c r="B338">
+        <v>8794.6550000000007</v>
+      </c>
+      <c r="C338">
+        <v>9806.59</v>
+      </c>
+      <c r="D338">
+        <v>340.33</v>
+      </c>
+      <c r="E338">
+        <v>4126.91</v>
+      </c>
+      <c r="F338">
+        <v>145.22999999999999</v>
+      </c>
+      <c r="G338">
+        <v>103.74890000000001</v>
+      </c>
+      <c r="H338">
+        <v>163.49</v>
+      </c>
+      <c r="I338">
+        <v>86.308899999999994</v>
+      </c>
+      <c r="J338">
+        <v>88.054500000000004</v>
+      </c>
+      <c r="K338">
+        <v>123.2033</v>
+      </c>
+      <c r="L338">
+        <v>879.62</v>
+      </c>
+      <c r="M338">
+        <v>1117.8800000000001</v>
+      </c>
+      <c r="N338">
+        <v>275.6737</v>
+      </c>
+      <c r="O338">
+        <v>279.74</v>
+      </c>
+      <c r="P338">
+        <v>353.28</v>
+      </c>
+      <c r="Q338">
+        <v>332.69</v>
+      </c>
+      <c r="R338">
+        <v>166.95</v>
+      </c>
+    </row>
+    <row r="339" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A339" s="1">
+        <v>45027</v>
+      </c>
+      <c r="B339">
+        <v>8794.2880000000005</v>
+      </c>
+      <c r="C339">
+        <v>9860.84</v>
+      </c>
+      <c r="D339">
+        <v>341.8</v>
+      </c>
+      <c r="E339">
+        <v>4139.0600000000004</v>
+      </c>
+      <c r="F339">
+        <v>145.61000000000001</v>
+      </c>
+      <c r="G339">
+        <v>103.69799999999999</v>
+      </c>
+      <c r="H339">
+        <v>163.38</v>
+      </c>
+      <c r="I339">
+        <v>86.287000000000006</v>
+      </c>
+      <c r="J339">
+        <v>88.035300000000007</v>
+      </c>
+      <c r="K339">
+        <v>123.19029999999999</v>
+      </c>
+      <c r="L339">
+        <v>879.7</v>
+      </c>
+      <c r="M339">
+        <v>1116.58</v>
+      </c>
+      <c r="N339">
+        <v>275.7029</v>
+      </c>
+      <c r="O339">
+        <v>279.93</v>
+      </c>
+      <c r="P339">
+        <v>353.34</v>
+      </c>
+      <c r="Q339">
+        <v>333.12</v>
+      </c>
+      <c r="R339">
+        <v>166.91</v>
+      </c>
+    </row>
+    <row r="340" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A340" s="1">
+        <v>45028</v>
+      </c>
+      <c r="B340">
+        <v>8758.1119999999992</v>
+      </c>
+      <c r="C340">
+        <v>9862.51</v>
+      </c>
+      <c r="D340">
+        <v>341.55</v>
+      </c>
+      <c r="E340">
+        <v>4135.43</v>
+      </c>
+      <c r="F340">
+        <v>145.19999999999999</v>
+      </c>
+      <c r="G340">
+        <v>103.4941</v>
+      </c>
+      <c r="H340">
+        <v>163.27000000000001</v>
+      </c>
+      <c r="I340">
+        <v>86.288700000000006</v>
+      </c>
+      <c r="J340">
+        <v>88.026600000000002</v>
+      </c>
+      <c r="K340">
+        <v>123.19240000000001</v>
+      </c>
+      <c r="L340">
+        <v>880.6</v>
+      </c>
+      <c r="M340">
+        <v>1116.05</v>
+      </c>
+      <c r="N340">
+        <v>275.74520000000001</v>
+      </c>
+      <c r="O340">
+        <v>280.64</v>
+      </c>
+      <c r="P340">
+        <v>354.14</v>
+      </c>
+      <c r="Q340">
+        <v>334.07</v>
+      </c>
+      <c r="R340">
+        <v>167.12</v>
+      </c>
+    </row>
+    <row r="341" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A341" s="1">
+        <v>45029</v>
+      </c>
+      <c r="B341">
+        <v>8875.6530000000002</v>
+      </c>
+      <c r="C341">
+        <v>9928.99</v>
+      </c>
+      <c r="D341">
+        <v>345.39</v>
+      </c>
+      <c r="E341">
+        <v>4118.17</v>
+      </c>
+      <c r="F341">
+        <v>143.63</v>
+      </c>
+      <c r="G341">
+        <v>103.7003</v>
+      </c>
+      <c r="H341">
+        <v>163.52000000000001</v>
+      </c>
+      <c r="I341">
+        <v>86.260599999999997</v>
+      </c>
+      <c r="J341">
+        <v>88.020099999999999</v>
+      </c>
+      <c r="K341">
+        <v>123.179</v>
+      </c>
+      <c r="L341">
+        <v>877.95</v>
+      </c>
+      <c r="M341">
+        <v>1116.06</v>
+      </c>
+      <c r="N341">
+        <v>275.76330000000002</v>
+      </c>
+      <c r="O341">
+        <v>279.99</v>
+      </c>
+      <c r="P341">
+        <v>353.5</v>
+      </c>
+      <c r="Q341">
+        <v>333.44</v>
+      </c>
+      <c r="R341">
+        <v>167.25</v>
+      </c>
+    </row>
+    <row r="342" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A342" s="1">
+        <v>45030</v>
+      </c>
+      <c r="B342">
+        <v>8857.3130000000001</v>
+      </c>
+      <c r="C342">
+        <v>9993.2000000000007</v>
+      </c>
+      <c r="D342">
+        <v>345.16</v>
+      </c>
+      <c r="E342">
+        <v>4095.08</v>
+      </c>
+      <c r="F342">
+        <v>141.86000000000001</v>
+      </c>
+      <c r="G342">
+        <v>103.5796</v>
+      </c>
+      <c r="H342">
+        <v>163.47</v>
+      </c>
+      <c r="I342">
+        <v>86.259500000000003</v>
+      </c>
+      <c r="J342">
+        <v>88.011300000000006</v>
+      </c>
+      <c r="K342">
+        <v>123.1778</v>
+      </c>
+      <c r="L342">
+        <v>878.53</v>
+      </c>
+      <c r="M342">
+        <v>1115.45</v>
+      </c>
+      <c r="N342">
+        <v>275.35050000000001</v>
+      </c>
+      <c r="O342">
+        <v>280.22000000000003</v>
+      </c>
+      <c r="P342">
+        <v>353.87</v>
+      </c>
+      <c r="Q342">
+        <v>333.88</v>
+      </c>
+      <c r="R342">
+        <v>167.59</v>
+      </c>
+    </row>
+    <row r="343" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A343" s="1">
+        <v>45033</v>
+      </c>
+      <c r="B343">
+        <v>8886.759</v>
+      </c>
+      <c r="C343">
+        <v>9940.5300000000007</v>
+      </c>
+      <c r="D343">
+        <v>345.45</v>
+      </c>
+      <c r="E343">
+        <v>4064.26</v>
+      </c>
+      <c r="F343">
+        <v>139.77000000000001</v>
+      </c>
+      <c r="G343">
+        <v>103.45140000000001</v>
+      </c>
+      <c r="H343">
+        <v>163.44</v>
+      </c>
+      <c r="I343">
+        <v>86.231800000000007</v>
+      </c>
+      <c r="J343">
+        <v>87.988299999999995</v>
+      </c>
+      <c r="K343">
+        <v>123.16459999999999</v>
+      </c>
+      <c r="L343">
+        <v>878.08</v>
+      </c>
+      <c r="M343">
+        <v>1113.82</v>
+      </c>
+      <c r="N343">
+        <v>275.53949999999998</v>
+      </c>
+      <c r="O343">
+        <v>280.37</v>
+      </c>
+      <c r="P343">
+        <v>354.03</v>
+      </c>
+      <c r="Q343">
+        <v>334.1</v>
+      </c>
+      <c r="R343">
+        <v>167.72</v>
+      </c>
+    </row>
+    <row r="344" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A344" s="1">
+        <v>45034</v>
+      </c>
+      <c r="B344">
+        <v>8894.3529999999992</v>
+      </c>
+      <c r="C344">
+        <v>10000.469999999999</v>
+      </c>
+      <c r="D344">
+        <v>346.28</v>
+      </c>
+      <c r="E344">
+        <v>4083.21</v>
+      </c>
+      <c r="F344">
+        <v>140.5</v>
+      </c>
+      <c r="G344">
+        <v>103.55540000000001</v>
+      </c>
+      <c r="H344">
+        <v>163.54</v>
+      </c>
+      <c r="I344">
+        <v>86.226900000000001</v>
+      </c>
+      <c r="J344">
+        <v>87.983599999999996</v>
+      </c>
+      <c r="K344">
+        <v>123.1611</v>
+      </c>
+      <c r="L344">
+        <v>877.98</v>
+      </c>
+      <c r="M344">
+        <v>1113.23</v>
+      </c>
+      <c r="N344">
+        <v>275.52409999999998</v>
+      </c>
+      <c r="O344">
+        <v>280.47000000000003</v>
+      </c>
+      <c r="P344">
+        <v>354.03</v>
+      </c>
+      <c r="Q344">
+        <v>334.31</v>
+      </c>
+      <c r="R344">
+        <v>167.78</v>
+      </c>
+    </row>
+    <row r="345" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A345" s="1">
+        <v>45035</v>
+      </c>
+      <c r="B345">
+        <v>8893.6020000000008</v>
+      </c>
+      <c r="C345">
+        <v>9999.6</v>
+      </c>
+      <c r="D345">
+        <v>345.63</v>
+      </c>
+      <c r="E345">
+        <v>4070.77</v>
+      </c>
+      <c r="F345">
+        <v>140.36000000000001</v>
+      </c>
+      <c r="G345">
+        <v>103.6009</v>
+      </c>
+      <c r="H345">
+        <v>163.85</v>
+      </c>
+      <c r="I345">
+        <v>86.224299999999999</v>
+      </c>
+      <c r="J345">
+        <v>87.982600000000005</v>
+      </c>
+      <c r="K345">
+        <v>123.1598</v>
+      </c>
+      <c r="L345">
+        <v>877.98</v>
+      </c>
+      <c r="M345">
+        <v>1113.33</v>
+      </c>
+      <c r="N345">
+        <v>275.53179999999998</v>
+      </c>
+      <c r="O345">
+        <v>280.62</v>
+      </c>
+      <c r="P345">
+        <v>354.25</v>
+      </c>
+      <c r="Q345">
+        <v>334.48</v>
+      </c>
+      <c r="R345">
+        <v>167.79</v>
+      </c>
+    </row>
+    <row r="346" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A346" s="1">
+        <v>45036</v>
+      </c>
+      <c r="B346">
+        <v>8841.616</v>
+      </c>
+      <c r="C346">
+        <v>9979.7900000000009</v>
+      </c>
+      <c r="D346">
+        <v>344.45</v>
+      </c>
+      <c r="E346">
+        <v>4088.39</v>
+      </c>
+      <c r="F346">
+        <v>141.81</v>
+      </c>
+      <c r="G346">
+        <v>103.6161</v>
+      </c>
+      <c r="H346">
+        <v>163.91</v>
+      </c>
+      <c r="I346">
+        <v>86.230599999999995</v>
+      </c>
+      <c r="J346">
+        <v>87.984099999999998</v>
+      </c>
+      <c r="K346">
+        <v>123.16240000000001</v>
+      </c>
+      <c r="L346">
+        <v>878.83</v>
+      </c>
+      <c r="M346">
+        <v>1114.3900000000001</v>
+      </c>
+      <c r="N346">
+        <v>275.50889999999998</v>
+      </c>
+      <c r="O346">
+        <v>280.81</v>
+      </c>
+      <c r="P346">
+        <v>354.43</v>
+      </c>
+      <c r="Q346">
+        <v>334.45</v>
+      </c>
+      <c r="R346">
+        <v>167.87</v>
+      </c>
+    </row>
+    <row r="347" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A347" s="1">
+        <v>45037</v>
+      </c>
+      <c r="B347">
+        <v>8849.76</v>
+      </c>
+      <c r="C347">
+        <v>10033.799999999999</v>
+      </c>
+      <c r="D347">
+        <v>344.17</v>
+      </c>
+      <c r="E347">
+        <v>4079.5</v>
+      </c>
+      <c r="F347">
+        <v>140.81</v>
+      </c>
+      <c r="G347">
+        <v>103.6056</v>
+      </c>
+      <c r="H347">
+        <v>163.92</v>
+      </c>
+      <c r="I347">
+        <v>86.224000000000004</v>
+      </c>
+      <c r="J347">
+        <v>87.984899999999996</v>
+      </c>
+      <c r="K347">
+        <v>123.1627</v>
+      </c>
+      <c r="L347">
+        <v>878.89</v>
+      </c>
+      <c r="M347">
+        <v>1113.1300000000001</v>
+      </c>
+      <c r="N347">
+        <v>275.71730000000002</v>
+      </c>
+      <c r="O347">
+        <v>280.94</v>
+      </c>
+      <c r="P347">
+        <v>354.79</v>
+      </c>
+      <c r="Q347">
+        <v>334.88</v>
+      </c>
+      <c r="R347">
+        <v>167.91</v>
+      </c>
+    </row>
+    <row r="348" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A348" s="1">
+        <v>45040</v>
+      </c>
+      <c r="B348">
+        <v>8857.3029999999999</v>
+      </c>
+      <c r="C348">
+        <v>10031.66</v>
+      </c>
+      <c r="D348">
+        <v>344.52</v>
+      </c>
+      <c r="E348">
+        <v>4111.66</v>
+      </c>
+      <c r="F348">
+        <v>142.51</v>
+      </c>
+      <c r="G348">
+        <v>103.6698</v>
+      </c>
+      <c r="H348">
+        <v>163.86</v>
+      </c>
+      <c r="I348">
+        <v>86.219099999999997</v>
+      </c>
+      <c r="J348">
+        <v>87.978200000000001</v>
+      </c>
+      <c r="K348">
+        <v>123.1588</v>
+      </c>
+      <c r="L348">
+        <v>878.88</v>
+      </c>
+      <c r="M348">
+        <v>1112.78</v>
+      </c>
+      <c r="N348">
+        <v>275.70389999999998</v>
+      </c>
+      <c r="O348">
+        <v>281.26</v>
+      </c>
+      <c r="P348">
+        <v>355</v>
+      </c>
+      <c r="Q348">
+        <v>335.28</v>
+      </c>
+      <c r="R348">
+        <v>167.98</v>
+      </c>
+    </row>
+    <row r="349" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A349" s="1">
+        <v>45041</v>
+      </c>
+      <c r="B349">
+        <v>8717.6309999999994</v>
+      </c>
+      <c r="C349">
+        <v>9989.26</v>
+      </c>
+      <c r="D349">
+        <v>340.06</v>
+      </c>
+      <c r="E349">
+        <v>4146.2</v>
+      </c>
+      <c r="F349">
+        <v>145.11000000000001</v>
+      </c>
+      <c r="G349">
+        <v>103.67230000000001</v>
+      </c>
+      <c r="H349">
+        <v>163.47999999999999</v>
+      </c>
+      <c r="I349">
+        <v>86.258899999999997</v>
+      </c>
+      <c r="J349">
+        <v>88.014799999999994</v>
+      </c>
+      <c r="K349">
+        <v>123.1773</v>
+      </c>
+      <c r="L349">
+        <v>881.46</v>
+      </c>
+      <c r="M349">
+        <v>1113.71</v>
+      </c>
+      <c r="N349">
+        <v>275.74520000000001</v>
+      </c>
+      <c r="O349">
+        <v>280.24</v>
+      </c>
+      <c r="P349">
+        <v>353.28</v>
+      </c>
+      <c r="Q349">
+        <v>334.64</v>
+      </c>
+      <c r="R349">
+        <v>167.92</v>
+      </c>
+    </row>
+    <row r="350" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A350" s="1">
+        <v>45042</v>
+      </c>
+      <c r="B350">
+        <v>8684.1910000000007</v>
+      </c>
+      <c r="C350">
+        <v>9927.85</v>
+      </c>
+      <c r="D350">
+        <v>339.11</v>
+      </c>
+      <c r="E350">
+        <v>4115.32</v>
+      </c>
+      <c r="F350">
+        <v>143.18</v>
+      </c>
+      <c r="G350">
+        <v>103.1491</v>
+      </c>
+      <c r="H350">
+        <v>163.12</v>
+      </c>
+      <c r="I350">
+        <v>86.233400000000003</v>
+      </c>
+      <c r="J350">
+        <v>88.005099999999999</v>
+      </c>
+      <c r="K350">
+        <v>123.16670000000001</v>
+      </c>
+      <c r="L350">
+        <v>882.87</v>
+      </c>
+      <c r="M350">
+        <v>1115.96</v>
+      </c>
+      <c r="N350">
+        <v>275.76850000000002</v>
+      </c>
+      <c r="O350">
+        <v>280.75</v>
+      </c>
+      <c r="P350">
+        <v>353.98</v>
+      </c>
+      <c r="Q350">
+        <v>334.98</v>
+      </c>
+      <c r="R350">
+        <v>168.42</v>
+      </c>
+    </row>
+    <row r="351" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A351" s="1">
+        <v>45043</v>
+      </c>
+      <c r="B351">
+        <v>8854.32</v>
+      </c>
+      <c r="C351">
+        <v>9955.7800000000007</v>
+      </c>
+      <c r="D351">
+        <v>343.23</v>
+      </c>
+      <c r="E351">
+        <v>4093.43</v>
+      </c>
+      <c r="F351">
+        <v>141.4</v>
+      </c>
+      <c r="G351">
+        <v>103.5608</v>
+      </c>
+      <c r="H351">
+        <v>163.63999999999999</v>
+      </c>
+      <c r="I351">
+        <v>86.131100000000004</v>
+      </c>
+      <c r="J351">
+        <v>87.878500000000003</v>
+      </c>
+      <c r="K351">
+        <v>123.11969999999999</v>
+      </c>
+      <c r="L351">
+        <v>878.28</v>
+      </c>
+      <c r="M351">
+        <v>1116.8800000000001</v>
+      </c>
+      <c r="N351">
+        <v>274.54180000000002</v>
+      </c>
+      <c r="O351">
+        <v>280.27</v>
+      </c>
+      <c r="P351">
+        <v>353.59</v>
+      </c>
+      <c r="Q351">
+        <v>334.74</v>
+      </c>
+      <c r="R351">
+        <v>168.41</v>
+      </c>
+    </row>
+    <row r="352" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A352" s="1">
+        <v>45044</v>
+      </c>
+      <c r="B352">
+        <v>8928.35</v>
+      </c>
+      <c r="C352">
+        <v>9967.69</v>
+      </c>
+      <c r="D352">
+        <v>345.7</v>
+      </c>
+      <c r="E352">
+        <v>4135.75</v>
+      </c>
+      <c r="F352">
+        <v>144.24</v>
+      </c>
+      <c r="G352">
+        <v>103.70740000000001</v>
+      </c>
+      <c r="H352">
+        <v>163.78</v>
+      </c>
+      <c r="I352">
+        <v>86.105099999999993</v>
+      </c>
+      <c r="J352">
+        <v>87.856099999999998</v>
+      </c>
+      <c r="K352">
+        <v>123.1079</v>
+      </c>
+      <c r="L352">
+        <v>876.84</v>
+      </c>
+      <c r="M352">
+        <v>1112.46</v>
+      </c>
+      <c r="N352">
+        <v>273.44549999999998</v>
+      </c>
+      <c r="O352">
+        <v>280.25</v>
+      </c>
+      <c r="P352">
+        <v>353.71</v>
+      </c>
+      <c r="Q352">
+        <v>334.97</v>
+      </c>
+      <c r="R352">
+        <v>168.26</v>
+      </c>
+    </row>
+    <row r="353" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A353" s="1">
+        <v>45047</v>
+      </c>
+      <c r="B353">
+        <v>8924.9189999999999</v>
+      </c>
+      <c r="C353">
+        <v>9967.69</v>
+      </c>
+      <c r="D353">
+        <v>345.44</v>
+      </c>
+      <c r="E353">
+        <v>4042.19</v>
+      </c>
+      <c r="F353">
+        <v>138.93</v>
+      </c>
+      <c r="G353">
+        <v>103.508</v>
+      </c>
+      <c r="H353">
+        <v>163.63999999999999</v>
+      </c>
+      <c r="I353">
+        <v>86.0886</v>
+      </c>
+      <c r="J353">
+        <v>87.829700000000003</v>
+      </c>
+      <c r="K353">
+        <v>123.095</v>
+      </c>
+      <c r="L353">
+        <v>877.09</v>
+      </c>
+      <c r="M353">
+        <v>1113.19</v>
+      </c>
+      <c r="N353">
+        <v>273.37090000000001</v>
+      </c>
+      <c r="O353">
+        <v>280.62</v>
+      </c>
+      <c r="P353">
+        <v>354</v>
+      </c>
+      <c r="Q353">
+        <v>335.49</v>
+      </c>
+      <c r="R353">
+        <v>168.44</v>
+      </c>
+    </row>
+    <row r="354" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A354" s="1">
+        <v>45048</v>
+      </c>
+      <c r="B354">
+        <v>8821.5930000000008</v>
+      </c>
+      <c r="C354">
+        <v>9827.39</v>
+      </c>
+      <c r="D354">
+        <v>342.03</v>
+      </c>
+      <c r="E354">
+        <v>4105.6899999999996</v>
+      </c>
+      <c r="F354">
+        <v>143.16</v>
+      </c>
+      <c r="G354">
+        <v>103.3488</v>
+      </c>
+      <c r="H354">
+        <v>163.46</v>
+      </c>
+      <c r="I354">
+        <v>86.107799999999997</v>
+      </c>
+      <c r="J354">
+        <v>87.854399999999998</v>
+      </c>
+      <c r="K354">
+        <v>123.1093</v>
+      </c>
+      <c r="L354">
+        <v>878.36</v>
+      </c>
+      <c r="M354">
+        <v>1114.93</v>
+      </c>
+      <c r="N354">
+        <v>273.51760000000002</v>
+      </c>
+      <c r="O354">
+        <v>279.19</v>
+      </c>
+      <c r="P354">
+        <v>352.05</v>
+      </c>
+      <c r="Q354">
+        <v>334.21</v>
+      </c>
+      <c r="R354">
+        <v>168.12</v>
+      </c>
+    </row>
+    <row r="355" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A355" s="1">
+        <v>45049</v>
+      </c>
+      <c r="B355">
+        <v>8759.9539999999997</v>
+      </c>
+      <c r="C355">
+        <v>9863.9699999999993</v>
+      </c>
+      <c r="D355">
+        <v>341.15</v>
+      </c>
+      <c r="E355">
+        <v>4119.26</v>
+      </c>
+      <c r="F355">
+        <v>144.24</v>
+      </c>
+      <c r="G355">
+        <v>103.23860000000001</v>
+      </c>
+      <c r="H355">
+        <v>163.33000000000001</v>
+      </c>
+      <c r="I355">
+        <v>86.093599999999995</v>
+      </c>
+      <c r="J355">
+        <v>87.832099999999997</v>
+      </c>
+      <c r="K355">
+        <v>123.07689999999999</v>
+      </c>
+      <c r="L355">
+        <v>879.67</v>
+      </c>
+      <c r="M355">
+        <v>1116.22</v>
+      </c>
+      <c r="N355">
+        <v>273.0625</v>
+      </c>
+      <c r="O355">
+        <v>279.58999999999997</v>
+      </c>
+      <c r="P355">
+        <v>352.47</v>
+      </c>
+      <c r="Q355">
+        <v>334.95</v>
+      </c>
+      <c r="R355">
+        <v>168.02</v>
+      </c>
+    </row>
+    <row r="356" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A356" s="1">
+        <v>45050</v>
+      </c>
+      <c r="B356">
+        <v>8697.6749999999993</v>
+      </c>
+      <c r="C356">
+        <v>9820.59</v>
+      </c>
+      <c r="D356">
+        <v>339.61</v>
+      </c>
+      <c r="E356">
+        <v>4081.57</v>
+      </c>
+      <c r="F356">
+        <v>142.11000000000001</v>
+      </c>
+      <c r="G356">
+        <v>103.29989999999999</v>
+      </c>
+      <c r="H356">
+        <v>163.35</v>
+      </c>
+      <c r="I356">
+        <v>86.203000000000003</v>
+      </c>
+      <c r="J356">
+        <v>87.942499999999995</v>
+      </c>
+      <c r="K356">
+        <v>123.1421</v>
+      </c>
+      <c r="L356">
+        <v>881.04</v>
+      </c>
+      <c r="M356">
+        <v>1117.93</v>
+      </c>
+      <c r="N356">
+        <v>272.6293</v>
+      </c>
+      <c r="O356">
+        <v>280.08999999999997</v>
+      </c>
+      <c r="P356">
+        <v>352.84</v>
+      </c>
+      <c r="Q356">
+        <v>334.91</v>
+      </c>
+      <c r="R356">
+        <v>167.8</v>
+      </c>
+    </row>
+    <row r="357" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A357" s="1">
+        <v>45051</v>
+      </c>
+      <c r="B357">
+        <v>8858.8590000000004</v>
+      </c>
+      <c r="C357">
+        <v>9958.2900000000009</v>
+      </c>
+      <c r="D357">
+        <v>344.51</v>
+      </c>
+      <c r="E357">
+        <v>4074.88</v>
+      </c>
+      <c r="F357">
+        <v>141.51</v>
+      </c>
+      <c r="G357">
+        <v>103.51860000000001</v>
+      </c>
+      <c r="H357">
+        <v>163.59</v>
+      </c>
+      <c r="I357">
+        <v>85.818799999999996</v>
+      </c>
+      <c r="J357">
+        <v>87.636899999999997</v>
+      </c>
+      <c r="K357">
+        <v>122.9269</v>
+      </c>
+      <c r="L357">
+        <v>876.48</v>
+      </c>
+      <c r="M357">
+        <v>1113.03</v>
+      </c>
+      <c r="N357">
+        <v>273.76330000000002</v>
+      </c>
+      <c r="O357">
+        <v>279.55</v>
+      </c>
+      <c r="P357">
+        <v>352.65</v>
+      </c>
+      <c r="Q357">
+        <v>335.11</v>
+      </c>
+      <c r="R357">
+        <v>167.69</v>
+      </c>
+    </row>
+    <row r="358" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A358" s="1">
+        <v>45054</v>
+      </c>
+      <c r="B358">
+        <v>8863.009</v>
+      </c>
+      <c r="C358">
+        <v>9989.18</v>
+      </c>
+      <c r="D358">
+        <v>345.43</v>
+      </c>
+      <c r="E358">
+        <v>4029.74</v>
+      </c>
+      <c r="F358">
+        <v>139.01</v>
+      </c>
+      <c r="G358">
+        <v>103.4579</v>
+      </c>
+      <c r="H358">
+        <v>163.53</v>
+      </c>
+      <c r="I358">
+        <v>85.796700000000001</v>
+      </c>
+      <c r="J358">
+        <v>87.614199999999997</v>
+      </c>
+      <c r="K358">
+        <v>122.9126</v>
+      </c>
+      <c r="L358">
+        <v>876.58</v>
+      </c>
+      <c r="M358">
+        <v>1111.43</v>
+      </c>
+      <c r="N358">
+        <v>273.39819999999997</v>
+      </c>
+      <c r="O358">
+        <v>279.64999999999998</v>
+      </c>
+      <c r="P358">
+        <v>352.84</v>
+      </c>
+      <c r="Q358">
+        <v>335.4</v>
+      </c>
+      <c r="R358">
+        <v>167.95</v>
+      </c>
+    </row>
+    <row r="359" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A359" s="1">
+        <v>45055</v>
+      </c>
+      <c r="B359">
+        <v>8823.0480000000007</v>
+      </c>
+      <c r="C359">
+        <v>9937.85</v>
+      </c>
+      <c r="D359">
+        <v>343.89</v>
+      </c>
+      <c r="E359">
+        <v>4024.27</v>
+      </c>
+      <c r="F359">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="G359">
+        <v>103.32380000000001</v>
+      </c>
+      <c r="H359">
+        <v>163.47</v>
+      </c>
+      <c r="I359">
+        <v>85.801699999999997</v>
+      </c>
+      <c r="J359">
+        <v>87.6096</v>
+      </c>
+      <c r="K359">
+        <v>122.91630000000001</v>
+      </c>
+      <c r="L359">
+        <v>877.44</v>
+      </c>
+      <c r="M359">
+        <v>1110.6400000000001</v>
+      </c>
+      <c r="N359">
+        <v>273.48340000000002</v>
+      </c>
+      <c r="O359">
+        <v>279.68</v>
+      </c>
+      <c r="P359">
+        <v>352.74</v>
+      </c>
+      <c r="Q359">
+        <v>335.53</v>
+      </c>
+      <c r="R359">
+        <v>167.9</v>
+      </c>
+    </row>
+    <row r="360" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A360" s="1">
+        <v>45056</v>
+      </c>
+      <c r="B360">
+        <v>8862.8520000000008</v>
+      </c>
+      <c r="C360">
+        <v>9900.32</v>
+      </c>
+      <c r="D360">
+        <v>344.6</v>
+      </c>
+      <c r="E360">
+        <v>4059.27</v>
+      </c>
+      <c r="F360">
+        <v>139.88999999999999</v>
+      </c>
+      <c r="G360">
+        <v>103.3441</v>
+      </c>
+      <c r="H360">
+        <v>163.44999999999999</v>
+      </c>
+      <c r="I360">
+        <v>85.776700000000005</v>
+      </c>
+      <c r="J360">
+        <v>87.5869</v>
+      </c>
+      <c r="K360">
+        <v>122.9062</v>
+      </c>
+      <c r="L360">
+        <v>876.72</v>
+      </c>
+      <c r="M360">
+        <v>1111.76</v>
+      </c>
+      <c r="N360">
+        <v>273.62110000000001</v>
+      </c>
+      <c r="O360">
+        <v>279.85000000000002</v>
+      </c>
+      <c r="P360">
+        <v>353.04</v>
+      </c>
+      <c r="Q360">
+        <v>335.8</v>
+      </c>
+      <c r="R360">
+        <v>168.18</v>
+      </c>
+    </row>
+    <row r="361" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A361" s="1">
+        <v>45057</v>
+      </c>
+      <c r="B361">
+        <v>8849.6919999999991</v>
+      </c>
+      <c r="C361">
+        <v>9911.48</v>
+      </c>
+      <c r="D361">
+        <v>343.78</v>
+      </c>
+      <c r="E361">
+        <v>4088.42</v>
+      </c>
+      <c r="F361">
+        <v>141.83000000000001</v>
+      </c>
+      <c r="G361">
+        <v>103.16370000000001</v>
+      </c>
+      <c r="H361">
+        <v>163.30000000000001</v>
+      </c>
+      <c r="I361">
+        <v>85.764499999999998</v>
+      </c>
+      <c r="J361">
+        <v>87.586299999999994</v>
+      </c>
+      <c r="K361">
+        <v>122.8998</v>
+      </c>
+      <c r="L361">
+        <v>877.2</v>
+      </c>
+      <c r="M361">
+        <v>1114.05</v>
+      </c>
+      <c r="N361">
+        <v>273.63589999999999</v>
+      </c>
+      <c r="O361">
+        <v>279.95</v>
+      </c>
+      <c r="P361">
+        <v>353.15</v>
+      </c>
+      <c r="Q361">
+        <v>335.81</v>
+      </c>
+      <c r="R361">
+        <v>168.47</v>
+      </c>
+    </row>
+    <row r="362" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A362" s="1">
+        <v>45058</v>
+      </c>
+      <c r="B362">
+        <v>8837.6839999999993</v>
+      </c>
+      <c r="C362">
+        <v>9941.91</v>
+      </c>
+      <c r="D362">
+        <v>343.07</v>
+      </c>
+      <c r="E362">
+        <v>4059.89</v>
+      </c>
+      <c r="F362">
+        <v>140.52000000000001</v>
+      </c>
+      <c r="G362">
+        <v>103.13200000000001</v>
+      </c>
+      <c r="H362">
+        <v>163.38</v>
+      </c>
+      <c r="I362">
+        <v>85.765000000000001</v>
+      </c>
+      <c r="J362">
+        <v>87.538200000000003</v>
+      </c>
+      <c r="K362">
+        <v>122.89019999999999</v>
+      </c>
+      <c r="L362">
+        <v>877.59</v>
+      </c>
+      <c r="M362">
+        <v>1112.99</v>
+      </c>
+      <c r="N362">
+        <v>273.7013</v>
+      </c>
+      <c r="O362">
+        <v>280.06</v>
+      </c>
+      <c r="P362">
+        <v>353.32</v>
+      </c>
+      <c r="Q362">
+        <v>335.97</v>
+      </c>
+      <c r="R362">
+        <v>168.59</v>
+      </c>
+    </row>
+    <row r="363" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A363" s="1">
+        <v>45061</v>
+      </c>
+      <c r="B363">
+        <v>8865.0290000000005</v>
+      </c>
+      <c r="C363">
+        <v>9942.25</v>
+      </c>
+      <c r="D363">
+        <v>344.39</v>
+      </c>
+      <c r="E363">
+        <v>4021.96</v>
+      </c>
+      <c r="F363">
+        <v>138.47</v>
+      </c>
+      <c r="G363">
+        <v>103.0714</v>
+      </c>
+      <c r="H363">
+        <v>163.29</v>
+      </c>
+      <c r="I363">
+        <v>85.730800000000002</v>
+      </c>
+      <c r="J363">
+        <v>87.5137</v>
+      </c>
+      <c r="K363">
+        <v>122.8742</v>
+      </c>
+      <c r="L363">
+        <v>877.11</v>
+      </c>
+      <c r="M363">
+        <v>1111.21</v>
+      </c>
+      <c r="N363">
+        <v>273.75290000000001</v>
+      </c>
+      <c r="O363">
+        <v>280.29000000000002</v>
+      </c>
+      <c r="P363">
+        <v>353.41</v>
+      </c>
+      <c r="Q363">
+        <v>336.09</v>
+      </c>
+      <c r="R363">
+        <v>168.6</v>
+      </c>
+    </row>
+    <row r="364" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A364" s="1">
+        <v>45062</v>
+      </c>
+      <c r="B364">
+        <v>8808.9480000000003</v>
+      </c>
+      <c r="C364">
+        <v>9940.19</v>
+      </c>
+      <c r="D364">
+        <v>342.62</v>
+      </c>
+      <c r="E364">
+        <v>3999.08</v>
+      </c>
+      <c r="F364">
+        <v>137.82</v>
+      </c>
+      <c r="G364">
+        <v>103.035</v>
+      </c>
+      <c r="H364">
+        <v>163.16999999999999</v>
+      </c>
+      <c r="I364">
+        <v>85.733900000000006</v>
+      </c>
+      <c r="J364">
+        <v>87.508099999999999</v>
+      </c>
+      <c r="K364">
+        <v>122.8745</v>
+      </c>
+      <c r="L364">
+        <v>878.19</v>
+      </c>
+      <c r="M364">
+        <v>1111.42</v>
+      </c>
+      <c r="N364">
+        <v>273.95170000000002</v>
+      </c>
+      <c r="O364">
+        <v>280.22000000000003</v>
+      </c>
+      <c r="P364">
+        <v>353.1</v>
+      </c>
+      <c r="Q364">
+        <v>336.22</v>
+      </c>
+      <c r="R364">
+        <v>168.7</v>
+      </c>
+    </row>
+    <row r="365" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A365" s="1">
+        <v>45063</v>
+      </c>
+      <c r="B365">
+        <v>8915.4310000000005</v>
+      </c>
+      <c r="C365">
+        <v>9959.58</v>
+      </c>
+      <c r="D365">
+        <v>344.55</v>
+      </c>
+      <c r="E365">
+        <v>3993.28</v>
+      </c>
+      <c r="F365">
+        <v>137.51</v>
+      </c>
+      <c r="G365">
+        <v>103.1793</v>
+      </c>
+      <c r="H365">
+        <v>163.44999999999999</v>
+      </c>
+      <c r="I365">
+        <v>85.717200000000005</v>
+      </c>
+      <c r="J365">
+        <v>87.499099999999999</v>
+      </c>
+      <c r="K365">
+        <v>122.8672</v>
+      </c>
+      <c r="L365">
+        <v>876.11</v>
+      </c>
+      <c r="M365">
+        <v>1110.81</v>
+      </c>
+      <c r="N365">
+        <v>274.2398</v>
+      </c>
+      <c r="O365">
+        <v>279.7</v>
+      </c>
+      <c r="P365">
+        <v>352.56</v>
+      </c>
+      <c r="Q365">
+        <v>335.63</v>
+      </c>
+      <c r="R365">
+        <v>168.66</v>
+      </c>
+    </row>
+    <row r="366" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A366" s="1">
+        <v>45064</v>
+      </c>
+      <c r="B366">
+        <v>9001.2510000000002</v>
+      </c>
+      <c r="C366">
+        <v>10063.42</v>
+      </c>
+      <c r="D366">
+        <v>346.8</v>
+      </c>
+      <c r="E366">
+        <v>3971.71</v>
+      </c>
+      <c r="F366">
+        <v>136.24</v>
+      </c>
+      <c r="G366">
+        <v>103.27809999999999</v>
+      </c>
+      <c r="H366">
+        <v>163.57</v>
+      </c>
+      <c r="I366">
+        <v>85.696799999999996</v>
+      </c>
+      <c r="J366">
+        <v>87.475999999999999</v>
+      </c>
+      <c r="K366">
+        <v>122.8539</v>
+      </c>
+      <c r="L366">
+        <v>874.76</v>
+      </c>
+      <c r="M366">
+        <v>1111.3800000000001</v>
+      </c>
+      <c r="N366">
+        <v>273.69630000000001</v>
+      </c>
+      <c r="O366">
+        <v>279.51</v>
+      </c>
+      <c r="P366">
+        <v>352.35</v>
+      </c>
+      <c r="Q366">
+        <v>335.21</v>
+      </c>
+      <c r="R366">
+        <v>168.55</v>
+      </c>
+    </row>
+    <row r="367" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A367" s="1">
+        <v>45065</v>
+      </c>
+      <c r="B367">
+        <v>8988.4590000000007</v>
+      </c>
+      <c r="C367">
+        <v>10127.59</v>
+      </c>
+      <c r="D367">
+        <v>347.08</v>
+      </c>
+      <c r="E367">
+        <v>3958.12</v>
+      </c>
+      <c r="F367">
+        <v>135.04</v>
+      </c>
+      <c r="G367">
+        <v>103.4526</v>
+      </c>
+      <c r="H367">
+        <v>163.75</v>
+      </c>
+      <c r="I367">
+        <v>85.703500000000005</v>
+      </c>
+      <c r="J367">
+        <v>87.468900000000005</v>
+      </c>
+      <c r="K367">
+        <v>122.8562</v>
+      </c>
+      <c r="L367">
+        <v>874.89</v>
+      </c>
+      <c r="M367">
+        <v>1110.5899999999999</v>
+      </c>
+      <c r="N367">
+        <v>273.99610000000001</v>
+      </c>
+      <c r="O367">
+        <v>279.82</v>
+      </c>
+      <c r="P367">
+        <v>352.73</v>
+      </c>
+      <c r="Q367">
+        <v>335.66</v>
+      </c>
+      <c r="R367">
+        <v>168.39</v>
+      </c>
+    </row>
+    <row r="368" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A368" s="1">
+        <v>45068</v>
+      </c>
+      <c r="B368">
+        <v>8990.8889999999992</v>
+      </c>
+      <c r="C368">
+        <v>10123.32</v>
+      </c>
+      <c r="D368">
+        <v>347.69</v>
+      </c>
+      <c r="E368">
+        <v>3955.27</v>
+      </c>
+      <c r="F368">
+        <v>134.38999999999999</v>
+      </c>
+      <c r="G368">
+        <v>103.39570000000001</v>
+      </c>
+      <c r="H368">
+        <v>163.82</v>
+      </c>
+      <c r="I368">
+        <v>85.695599999999999</v>
+      </c>
+      <c r="J368">
+        <v>87.461699999999993</v>
+      </c>
+      <c r="K368">
+        <v>122.85080000000001</v>
+      </c>
+      <c r="L368">
+        <v>874.86</v>
+      </c>
+      <c r="M368">
+        <v>1111.03</v>
+      </c>
+      <c r="N368">
+        <v>273.98809999999997</v>
+      </c>
+      <c r="O368">
+        <v>280.10000000000002</v>
+      </c>
+      <c r="P368">
+        <v>353.08</v>
+      </c>
+      <c r="Q368">
+        <v>336.15</v>
+      </c>
+      <c r="R368">
+        <v>168.39</v>
+      </c>
+    </row>
+    <row r="369" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A369" s="1">
+        <v>45069</v>
+      </c>
+      <c r="B369">
+        <v>8890.1560000000009</v>
+      </c>
+      <c r="C369">
+        <v>10023.51</v>
+      </c>
+      <c r="D369">
+        <v>344.4</v>
+      </c>
+      <c r="E369">
+        <v>3963.8</v>
+      </c>
+      <c r="F369">
+        <v>134.76</v>
+      </c>
+      <c r="G369">
+        <v>103.10209999999999</v>
+      </c>
+      <c r="H369">
+        <v>163.44</v>
+      </c>
+      <c r="I369">
+        <v>85.708100000000002</v>
+      </c>
+      <c r="J369">
+        <v>87.476500000000001</v>
+      </c>
+      <c r="K369">
+        <v>122.8573</v>
+      </c>
+      <c r="L369">
+        <v>876.38</v>
+      </c>
+      <c r="M369">
+        <v>1111.01</v>
+      </c>
+      <c r="N369">
+        <v>274.00069999999999</v>
+      </c>
+      <c r="O369">
+        <v>279.91000000000003</v>
+      </c>
+      <c r="P369">
+        <v>352.53</v>
+      </c>
+      <c r="Q369">
+        <v>336.05</v>
+      </c>
+      <c r="R369">
+        <v>168.5</v>
+      </c>
+    </row>
+    <row r="370" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A370" s="1">
+        <v>45070</v>
+      </c>
+      <c r="B370">
+        <v>8825.2620000000006</v>
+      </c>
+      <c r="C370">
+        <v>9841.99</v>
+      </c>
+      <c r="D370">
+        <v>341.05</v>
+      </c>
+      <c r="E370">
+        <v>3947.94</v>
+      </c>
+      <c r="F370">
+        <v>134.03</v>
+      </c>
+      <c r="G370">
+        <v>102.94280000000001</v>
+      </c>
+      <c r="H370">
+        <v>163.26</v>
+      </c>
+      <c r="I370">
+        <v>85.767499999999998</v>
+      </c>
+      <c r="J370">
+        <v>87.533100000000005</v>
+      </c>
+      <c r="K370">
+        <v>122.8927</v>
+      </c>
+      <c r="L370">
+        <v>877.38</v>
+      </c>
+      <c r="M370">
+        <v>1110.56</v>
+      </c>
+      <c r="N370">
+        <v>273.54579999999999</v>
+      </c>
+      <c r="O370">
+        <v>280.05</v>
+      </c>
+      <c r="P370">
+        <v>352.44</v>
+      </c>
+      <c r="Q370">
+        <v>336.48</v>
+      </c>
+      <c r="R370">
+        <v>168.28</v>
+      </c>
+    </row>
+    <row r="371" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A371" s="1">
+        <v>45071</v>
+      </c>
+      <c r="B371">
+        <v>8902.84</v>
+      </c>
+      <c r="C371">
+        <v>9855.58</v>
+      </c>
+      <c r="D371">
+        <v>341.68</v>
+      </c>
+      <c r="E371">
+        <v>3940.72</v>
+      </c>
+      <c r="F371">
+        <v>133.78</v>
+      </c>
+      <c r="G371">
+        <v>103.0534</v>
+      </c>
+      <c r="H371">
+        <v>163.57</v>
+      </c>
+      <c r="I371">
+        <v>85.692899999999995</v>
+      </c>
+      <c r="J371">
+        <v>87.452799999999996</v>
+      </c>
+      <c r="K371">
+        <v>122.8411</v>
+      </c>
+      <c r="L371">
+        <v>876.05</v>
+      </c>
+      <c r="M371">
+        <v>1121.44</v>
+      </c>
+      <c r="N371">
+        <v>273.91860000000003</v>
+      </c>
+      <c r="O371">
+        <v>279.95999999999998</v>
+      </c>
+      <c r="P371">
+        <v>352.32</v>
+      </c>
+      <c r="Q371">
+        <v>336.23</v>
+      </c>
+      <c r="R371">
+        <v>168.47</v>
+      </c>
+    </row>
+    <row r="372" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A372" s="1">
+        <v>45072</v>
+      </c>
+      <c r="B372">
+        <v>9019.6409999999996</v>
+      </c>
+      <c r="C372">
+        <v>10012.25</v>
+      </c>
+      <c r="D372">
+        <v>345.43</v>
+      </c>
+      <c r="E372">
+        <v>3950.84</v>
+      </c>
+      <c r="F372">
+        <v>134.35</v>
+      </c>
+      <c r="G372">
+        <v>103.3719</v>
+      </c>
+      <c r="H372">
+        <v>163.69</v>
+      </c>
+      <c r="I372">
+        <v>85.602800000000002</v>
+      </c>
+      <c r="J372">
+        <v>87.361099999999993</v>
+      </c>
+      <c r="K372">
+        <v>122.7838</v>
+      </c>
+      <c r="L372">
+        <v>873.96</v>
+      </c>
+      <c r="M372">
+        <v>1123.23</v>
+      </c>
+      <c r="N372">
+        <v>273.55860000000001</v>
+      </c>
+      <c r="O372">
+        <v>279.74</v>
+      </c>
+      <c r="P372">
+        <v>352.09</v>
+      </c>
+      <c r="Q372">
+        <v>335.81</v>
+      </c>
+      <c r="R372">
+        <v>168.28</v>
+      </c>
+    </row>
+    <row r="373" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A373" s="1">
+        <v>45075</v>
+      </c>
+      <c r="B373">
+        <v>9019.6409999999996</v>
+      </c>
+      <c r="C373">
+        <v>9971.86</v>
+      </c>
+      <c r="D373">
+        <v>345.66</v>
+      </c>
+      <c r="E373">
+        <v>3950.84</v>
+      </c>
+      <c r="F373">
+        <v>134.35</v>
+      </c>
+      <c r="G373">
+        <v>103.3719</v>
+      </c>
+      <c r="H373">
+        <v>163.69</v>
+      </c>
+      <c r="I373">
+        <v>85.602800000000002</v>
+      </c>
+      <c r="J373">
+        <v>87.361099999999993</v>
+      </c>
+      <c r="K373">
+        <v>122.7838</v>
+      </c>
+      <c r="L373">
+        <v>873.96</v>
+      </c>
+      <c r="M373">
+        <v>1123.23</v>
+      </c>
+      <c r="N373">
+        <v>273.55860000000001</v>
+      </c>
+      <c r="O373">
+        <v>279.74</v>
+      </c>
+      <c r="P373">
+        <v>352.09</v>
+      </c>
+      <c r="Q373">
+        <v>335.81</v>
+      </c>
+      <c r="R373">
+        <v>168.28</v>
+      </c>
+    </row>
+    <row r="374" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A374" s="1">
+        <v>45076</v>
+      </c>
+      <c r="B374">
+        <v>9020.3919999999998</v>
+      </c>
+      <c r="C374">
+        <v>9917.27</v>
+      </c>
+      <c r="D374">
+        <v>345.14</v>
+      </c>
+      <c r="E374">
+        <v>4001.23</v>
+      </c>
+      <c r="F374">
+        <v>136.91</v>
+      </c>
+      <c r="G374">
+        <v>103.1747</v>
+      </c>
+      <c r="H374">
+        <v>163.52000000000001</v>
+      </c>
+      <c r="I374">
+        <v>85.579499999999996</v>
+      </c>
+      <c r="J374">
+        <v>87.338999999999999</v>
+      </c>
+      <c r="K374">
+        <v>122.7739</v>
+      </c>
+      <c r="L374">
+        <v>874.31</v>
+      </c>
+      <c r="M374">
+        <v>1124.68</v>
+      </c>
+      <c r="N374">
+        <v>272.90359999999998</v>
+      </c>
+      <c r="O374">
+        <v>280.93</v>
+      </c>
+      <c r="P374">
+        <v>352.78</v>
+      </c>
+      <c r="Q374">
+        <v>337.07</v>
+      </c>
+      <c r="R374">
+        <v>168.4</v>
+      </c>
+    </row>
+    <row r="375" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A375" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B375">
+        <v>8967.1589999999997</v>
+      </c>
+      <c r="C375">
+        <v>9747.34</v>
+      </c>
+      <c r="D375">
+        <v>342</v>
+      </c>
+      <c r="E375">
+        <v>4020.88</v>
+      </c>
+      <c r="F375">
+        <v>138.65</v>
+      </c>
+      <c r="G375">
+        <v>102.8546</v>
+      </c>
+      <c r="H375">
+        <v>163.32</v>
+      </c>
+      <c r="I375">
+        <v>85.571700000000007</v>
+      </c>
+      <c r="J375">
+        <v>87.322800000000001</v>
+      </c>
+      <c r="K375">
+        <v>122.77070000000001</v>
+      </c>
+      <c r="L375">
+        <v>875.38</v>
+      </c>
+      <c r="M375">
+        <v>1127.3800000000001</v>
+      </c>
+      <c r="N375">
+        <v>273.34010000000001</v>
+      </c>
+      <c r="O375">
+        <v>281.17</v>
+      </c>
+      <c r="P375">
+        <v>352.97</v>
+      </c>
+      <c r="Q375">
+        <v>337.34</v>
+      </c>
+      <c r="R375">
+        <v>168.58</v>
+      </c>
+    </row>
+    <row r="376" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A376" s="1">
+        <v>45078</v>
+      </c>
+      <c r="B376">
+        <v>9057.1749999999993</v>
+      </c>
+      <c r="C376">
+        <v>9838.7800000000007</v>
+      </c>
+      <c r="D376">
+        <v>345.56</v>
+      </c>
+      <c r="E376">
+        <v>4036.72</v>
+      </c>
+      <c r="F376">
+        <v>139.11000000000001</v>
+      </c>
+      <c r="G376">
+        <v>102.7533</v>
+      </c>
+      <c r="H376">
+        <v>163.30000000000001</v>
+      </c>
+      <c r="I376">
+        <v>85.516499999999994</v>
+      </c>
+      <c r="J376">
+        <v>87.282499999999999</v>
+      </c>
+      <c r="K376">
+        <v>122.73609999999999</v>
+      </c>
+      <c r="L376">
+        <v>874.03</v>
+      </c>
+      <c r="M376">
+        <v>1124.49</v>
+      </c>
+      <c r="N376">
+        <v>273.65320000000003</v>
+      </c>
+      <c r="O376">
+        <v>280.64999999999998</v>
+      </c>
+      <c r="P376">
+        <v>352.53</v>
+      </c>
+      <c r="Q376">
+        <v>336.86</v>
+      </c>
+      <c r="R376">
+        <v>168.53</v>
+      </c>
+    </row>
+    <row r="377" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A377" s="1">
+        <v>45079</v>
+      </c>
+      <c r="B377">
+        <v>9189.3420000000006</v>
+      </c>
+      <c r="C377">
+        <v>9991.09</v>
+      </c>
+      <c r="D377">
+        <v>350.99</v>
+      </c>
+      <c r="E377">
+        <v>4018.68</v>
+      </c>
+      <c r="F377">
+        <v>137.44</v>
+      </c>
+      <c r="G377">
+        <v>102.91719999999999</v>
+      </c>
+      <c r="H377">
+        <v>163.55000000000001</v>
+      </c>
+      <c r="I377">
+        <v>85.502499999999998</v>
+      </c>
+      <c r="J377">
+        <v>87.259500000000003</v>
+      </c>
+      <c r="K377">
+        <v>122.7273</v>
+      </c>
+      <c r="L377">
+        <v>872.24</v>
+      </c>
+      <c r="M377">
+        <v>1120.3699999999999</v>
+      </c>
+      <c r="N377">
+        <v>272.5478</v>
+      </c>
+      <c r="O377">
+        <v>280.04000000000002</v>
+      </c>
+      <c r="P377">
+        <v>351.92</v>
+      </c>
+      <c r="Q377">
+        <v>336.42</v>
+      </c>
+      <c r="R377">
+        <v>168.21</v>
+      </c>
+    </row>
+    <row r="378" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A378" s="1">
+        <v>45082</v>
+      </c>
+      <c r="B378">
+        <v>9171.0910000000003</v>
+      </c>
+      <c r="C378">
+        <v>9921.1200000000008</v>
+      </c>
+      <c r="D378">
+        <v>350.76</v>
+      </c>
+      <c r="E378">
+        <v>4014.58</v>
+      </c>
+      <c r="F378">
+        <v>137.11000000000001</v>
+      </c>
+      <c r="G378">
+        <v>102.7548</v>
+      </c>
+      <c r="H378">
+        <v>163.44</v>
+      </c>
+      <c r="I378">
+        <v>85.501099999999994</v>
+      </c>
+      <c r="J378">
+        <v>87.257800000000003</v>
+      </c>
+      <c r="K378">
+        <v>122.7265</v>
+      </c>
+      <c r="L378">
+        <v>872.52</v>
+      </c>
+      <c r="M378">
+        <v>1118.3399999999999</v>
+      </c>
+      <c r="N378">
+        <v>271.84859999999998</v>
+      </c>
+      <c r="O378">
+        <v>280.08999999999997</v>
+      </c>
+      <c r="P378">
+        <v>352.14</v>
+      </c>
+      <c r="Q378">
+        <v>336.58</v>
+      </c>
+      <c r="R378">
+        <v>168.18</v>
+      </c>
+    </row>
+    <row r="379" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A379" s="1">
+        <v>45083</v>
+      </c>
+      <c r="B379">
+        <v>9192.9150000000009</v>
+      </c>
+      <c r="C379">
+        <v>9925.68</v>
+      </c>
+      <c r="D379">
+        <v>351.68</v>
+      </c>
+      <c r="E379">
+        <v>4027.2</v>
+      </c>
+      <c r="F379">
+        <v>138.22</v>
+      </c>
+      <c r="G379">
+        <v>102.4264</v>
+      </c>
+      <c r="H379">
+        <v>163.37</v>
+      </c>
+      <c r="I379">
+        <v>85.493200000000002</v>
+      </c>
+      <c r="J379">
+        <v>87.250200000000007</v>
+      </c>
+      <c r="K379">
+        <v>122.72190000000001</v>
+      </c>
+      <c r="L379">
+        <v>872.35</v>
+      </c>
+      <c r="M379">
+        <v>1117.3900000000001</v>
+      </c>
+      <c r="N379">
+        <v>272.30680000000001</v>
+      </c>
+      <c r="O379">
+        <v>280.11</v>
+      </c>
+      <c r="P379">
+        <v>352.09</v>
+      </c>
+      <c r="Q379">
+        <v>336.68</v>
+      </c>
+      <c r="R379">
+        <v>168.23</v>
+      </c>
+    </row>
+    <row r="380" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A380" s="1">
+        <v>45084</v>
+      </c>
+      <c r="B380">
+        <v>9158.1350000000002</v>
+      </c>
+      <c r="C380">
+        <v>9918.0400000000009</v>
+      </c>
+      <c r="D380">
+        <v>350.72</v>
+      </c>
+      <c r="E380">
+        <v>3981.12</v>
+      </c>
+      <c r="F380">
+        <v>135.55000000000001</v>
+      </c>
+      <c r="G380">
+        <v>102.2295</v>
+      </c>
+      <c r="H380">
+        <v>163.33000000000001</v>
+      </c>
+      <c r="I380">
+        <v>85.492699999999999</v>
+      </c>
+      <c r="J380">
+        <v>87.248599999999996</v>
+      </c>
+      <c r="K380">
+        <v>122.7216</v>
+      </c>
+      <c r="L380">
+        <v>872.77</v>
+      </c>
+      <c r="M380">
+        <v>1121.95</v>
+      </c>
+      <c r="N380">
+        <v>272.69690000000003</v>
+      </c>
+      <c r="O380">
+        <v>280.19</v>
+      </c>
+      <c r="P380">
+        <v>352.25</v>
+      </c>
+      <c r="Q380">
+        <v>336.77</v>
+      </c>
+      <c r="R380">
+        <v>168.44</v>
+      </c>
+    </row>
+    <row r="381" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A381" s="1">
+        <v>45085</v>
+      </c>
+      <c r="B381">
+        <v>9215.8649999999998</v>
+      </c>
+      <c r="C381">
+        <v>9931.3700000000008</v>
+      </c>
+      <c r="D381">
+        <v>352.4</v>
+      </c>
+      <c r="E381">
+        <v>4013.66</v>
+      </c>
+      <c r="F381">
+        <v>137.43</v>
+      </c>
+      <c r="G381">
+        <v>102.26349999999999</v>
+      </c>
+      <c r="H381">
+        <v>163.44</v>
+      </c>
+      <c r="I381">
+        <v>85.489800000000002</v>
+      </c>
+      <c r="J381">
+        <v>87.246200000000002</v>
+      </c>
+      <c r="K381">
+        <v>122.7196</v>
+      </c>
+      <c r="L381">
+        <v>872.1</v>
+      </c>
+      <c r="M381">
+        <v>1120.83</v>
+      </c>
+      <c r="N381">
+        <v>272.73880000000003</v>
+      </c>
+      <c r="O381">
+        <v>280.18</v>
+      </c>
+      <c r="P381">
+        <v>352.24</v>
+      </c>
+      <c r="Q381">
+        <v>336.55</v>
+      </c>
+      <c r="R381">
+        <v>168.42</v>
+      </c>
+    </row>
+    <row r="382" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A382" s="1">
+        <v>45086</v>
+      </c>
+      <c r="B382">
+        <v>9226.7000000000007</v>
+      </c>
+      <c r="C382">
+        <v>9913.15</v>
+      </c>
+      <c r="D382">
+        <v>353.11</v>
+      </c>
+      <c r="E382">
+        <v>4007.73</v>
+      </c>
+      <c r="F382">
+        <v>137.54</v>
+      </c>
+      <c r="G382">
+        <v>102.3116</v>
+      </c>
+      <c r="H382">
+        <v>163.47</v>
+      </c>
+      <c r="I382">
+        <v>85.490399999999994</v>
+      </c>
+      <c r="J382">
+        <v>87.245199999999997</v>
+      </c>
+      <c r="K382">
+        <v>122.7199</v>
+      </c>
+      <c r="L382">
+        <v>871.96</v>
+      </c>
+      <c r="M382">
+        <v>1119.54</v>
+      </c>
+      <c r="N382">
+        <v>272.76569999999998</v>
+      </c>
+      <c r="O382">
+        <v>280.3</v>
+      </c>
+      <c r="P382">
+        <v>352.41</v>
+      </c>
+      <c r="Q382">
+        <v>336.8</v>
+      </c>
+      <c r="R382">
+        <v>168.28</v>
+      </c>
+    </row>
+    <row r="383" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A383" s="1">
+        <v>45089</v>
+      </c>
+      <c r="B383">
+        <v>9312.7180000000008</v>
+      </c>
+      <c r="C383">
+        <v>9974.85</v>
+      </c>
+      <c r="D383">
+        <v>355.38</v>
+      </c>
+      <c r="E383">
+        <v>4019.37</v>
+      </c>
+      <c r="F383">
+        <v>137.94999999999999</v>
+      </c>
+      <c r="G383">
+        <v>102.5985</v>
+      </c>
+      <c r="H383">
+        <v>163.52000000000001</v>
+      </c>
+      <c r="I383">
+        <v>85.490099999999998</v>
+      </c>
+      <c r="J383">
+        <v>87.246099999999998</v>
+      </c>
+      <c r="K383">
+        <v>122.7197</v>
+      </c>
+      <c r="L383">
+        <v>871.04</v>
+      </c>
+      <c r="M383">
+        <v>1118.24</v>
+      </c>
+      <c r="N383">
+        <v>272.94869999999997</v>
+      </c>
+      <c r="O383">
+        <v>279.58</v>
+      </c>
+      <c r="P383">
+        <v>352.32</v>
+      </c>
+      <c r="Q383">
+        <v>336.45</v>
+      </c>
+      <c r="R383">
+        <v>168.04</v>
+      </c>
+    </row>
+    <row r="384" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A384" s="1">
+        <v>45090</v>
+      </c>
+      <c r="B384">
+        <v>9377.6489999999994</v>
+      </c>
+      <c r="C384">
+        <v>10046.620000000001</v>
+      </c>
+      <c r="D384">
+        <v>358.38</v>
+      </c>
+      <c r="E384">
+        <v>3997.91</v>
+      </c>
+      <c r="F384">
+        <v>136.32</v>
+      </c>
+      <c r="G384">
+        <v>102.87909999999999</v>
+      </c>
+      <c r="H384">
+        <v>163.55000000000001</v>
+      </c>
+      <c r="I384">
+        <v>85.488500000000002</v>
+      </c>
+      <c r="J384">
+        <v>87.242999999999995</v>
+      </c>
+      <c r="K384">
+        <v>122.71939999999999</v>
+      </c>
+      <c r="L384">
+        <v>870.5</v>
+      </c>
+      <c r="M384">
+        <v>1116.56</v>
+      </c>
+      <c r="N384">
+        <v>273.56169999999997</v>
+      </c>
+      <c r="O384">
+        <v>279.86</v>
+      </c>
+      <c r="P384">
+        <v>352.46</v>
+      </c>
+      <c r="Q384">
+        <v>336.79</v>
+      </c>
+      <c r="R384">
+        <v>167.85</v>
+      </c>
+    </row>
+    <row r="385" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A385" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B385">
+        <v>9387.5360000000001</v>
+      </c>
+      <c r="C385">
+        <v>10112.32</v>
+      </c>
+      <c r="D385">
+        <v>359.58</v>
+      </c>
+      <c r="E385">
+        <v>4019.32</v>
+      </c>
+      <c r="F385">
+        <v>137.86000000000001</v>
+      </c>
+      <c r="G385">
+        <v>102.76130000000001</v>
+      </c>
+      <c r="H385">
+        <v>163.5</v>
+      </c>
+      <c r="I385">
+        <v>85.482900000000001</v>
+      </c>
+      <c r="J385">
+        <v>87.239599999999996</v>
+      </c>
+      <c r="K385">
+        <v>122.7165</v>
+      </c>
+      <c r="L385">
+        <v>870.53</v>
+      </c>
+      <c r="M385">
+        <v>1119.95</v>
+      </c>
+      <c r="N385">
+        <v>273.05759999999998</v>
+      </c>
+      <c r="O385">
+        <v>280.52</v>
+      </c>
+      <c r="P385">
+        <v>353.34</v>
+      </c>
+      <c r="Q385">
+        <v>337.27</v>
+      </c>
+      <c r="R385">
+        <v>168.04</v>
+      </c>
+    </row>
+    <row r="386" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A386" s="1">
+        <v>45092</v>
+      </c>
+      <c r="B386">
+        <v>9503.5319999999992</v>
+      </c>
+      <c r="C386">
+        <v>10087.200000000001</v>
+      </c>
+      <c r="D386">
+        <v>362.89</v>
+      </c>
+      <c r="E386">
+        <v>4057.65</v>
+      </c>
+      <c r="F386">
+        <v>139.31</v>
+      </c>
+      <c r="G386">
+        <v>103.1724</v>
+      </c>
+      <c r="H386">
+        <v>163.72999999999999</v>
+      </c>
+      <c r="I386">
+        <v>85.4833</v>
+      </c>
+      <c r="J386">
+        <v>87.236400000000003</v>
+      </c>
+      <c r="K386">
+        <v>122.7154</v>
+      </c>
+      <c r="L386">
+        <v>869.52</v>
+      </c>
+      <c r="M386">
+        <v>1119.27</v>
+      </c>
+      <c r="N386">
+        <v>271.63670000000002</v>
+      </c>
+      <c r="O386">
+        <v>279.68</v>
+      </c>
+      <c r="P386">
+        <v>352.1</v>
+      </c>
+      <c r="Q386">
+        <v>335.79</v>
+      </c>
+      <c r="R386">
+        <v>167.83</v>
+      </c>
+    </row>
+    <row r="387" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A387" s="1">
+        <v>45093</v>
+      </c>
+      <c r="B387">
+        <v>9468.8080000000009</v>
+      </c>
+      <c r="C387">
+        <v>10155.85</v>
+      </c>
+      <c r="D387">
+        <v>362.7</v>
+      </c>
+      <c r="E387">
+        <v>4055.1</v>
+      </c>
+      <c r="F387">
+        <v>138.99</v>
+      </c>
+      <c r="G387">
+        <v>102.94629999999999</v>
+      </c>
+      <c r="H387">
+        <v>163.46</v>
+      </c>
+      <c r="I387">
+        <v>85.480800000000002</v>
+      </c>
+      <c r="J387">
+        <v>87.238600000000005</v>
+      </c>
+      <c r="K387">
+        <v>122.7153</v>
+      </c>
+      <c r="L387">
+        <v>869.82</v>
+      </c>
+      <c r="M387">
+        <v>1118.5</v>
+      </c>
+      <c r="N387">
+        <v>269.16059999999999</v>
+      </c>
+      <c r="O387">
+        <v>279.99</v>
+      </c>
+      <c r="P387">
+        <v>352.68</v>
+      </c>
+      <c r="Q387">
+        <v>336.42</v>
+      </c>
+      <c r="R387">
+        <v>167.96</v>
+      </c>
+    </row>
+    <row r="388" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A388" s="1">
+        <v>45096</v>
+      </c>
+      <c r="B388">
+        <v>9468.8080000000009</v>
+      </c>
+      <c r="C388">
+        <v>10080.879999999999</v>
+      </c>
+      <c r="D388">
+        <v>361.66</v>
+      </c>
+      <c r="E388">
+        <v>4055.1</v>
+      </c>
+      <c r="F388">
+        <v>138.99</v>
+      </c>
+      <c r="G388">
+        <v>102.94629999999999</v>
+      </c>
+      <c r="H388">
+        <v>163.46</v>
+      </c>
+      <c r="I388">
+        <v>85.480800000000002</v>
+      </c>
+      <c r="J388">
+        <v>87.238600000000005</v>
+      </c>
+      <c r="K388">
+        <v>122.7153</v>
+      </c>
+      <c r="L388">
+        <v>869.82</v>
+      </c>
+      <c r="M388">
+        <v>1118.5</v>
+      </c>
+      <c r="N388">
+        <v>269.16059999999999</v>
+      </c>
+      <c r="O388">
+        <v>279.99</v>
+      </c>
+      <c r="P388">
+        <v>352.68</v>
+      </c>
+      <c r="Q388">
+        <v>336.42</v>
+      </c>
+      <c r="R388">
+        <v>167.96</v>
+      </c>
+    </row>
+    <row r="389" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A389" s="1">
+        <v>45097</v>
+      </c>
+      <c r="B389">
+        <v>9424.0249999999996</v>
+      </c>
+      <c r="C389">
+        <v>10036.43</v>
+      </c>
+      <c r="D389">
+        <v>359.6</v>
+      </c>
+      <c r="E389">
+        <v>4078.64</v>
+      </c>
+      <c r="F389">
+        <v>140.19999999999999</v>
+      </c>
+      <c r="G389">
+        <v>102.86069999999999</v>
+      </c>
+      <c r="H389">
+        <v>163.46</v>
+      </c>
+      <c r="I389">
+        <v>85.480599999999995</v>
+      </c>
+      <c r="J389">
+        <v>87.235799999999998</v>
+      </c>
+      <c r="K389">
+        <v>122.715</v>
+      </c>
+      <c r="L389">
+        <v>870.2</v>
+      </c>
+      <c r="M389">
+        <v>1117.96</v>
+      </c>
+      <c r="N389">
+        <v>269.68049999999999</v>
+      </c>
+      <c r="O389">
+        <v>280.02999999999997</v>
+      </c>
+      <c r="P389">
+        <v>352.87</v>
+      </c>
+      <c r="Q389">
+        <v>336.63</v>
+      </c>
+      <c r="R389">
+        <v>167.98</v>
+      </c>
+    </row>
+    <row r="390" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A390" s="1">
+        <v>45098</v>
+      </c>
+      <c r="B390">
+        <v>9375.2080000000005</v>
+      </c>
+      <c r="C390">
+        <v>9993.76</v>
+      </c>
+      <c r="D390">
+        <v>357.99</v>
+      </c>
+      <c r="E390">
+        <v>4082.6</v>
+      </c>
+      <c r="F390">
+        <v>140.72999999999999</v>
+      </c>
+      <c r="G390">
+        <v>102.62390000000001</v>
+      </c>
+      <c r="H390">
+        <v>163.21</v>
+      </c>
+      <c r="I390">
+        <v>85.4739</v>
+      </c>
+      <c r="J390">
+        <v>87.229100000000003</v>
+      </c>
+      <c r="K390">
+        <v>122.71</v>
+      </c>
+      <c r="L390">
+        <v>870.63</v>
+      </c>
+      <c r="M390">
+        <v>1118.22</v>
+      </c>
+      <c r="N390">
+        <v>270.1044</v>
+      </c>
+      <c r="O390">
+        <v>280.07</v>
+      </c>
+      <c r="P390">
+        <v>352.88</v>
+      </c>
+      <c r="Q390">
+        <v>336.64</v>
+      </c>
+      <c r="R390">
+        <v>168.08</v>
+      </c>
+    </row>
+    <row r="391" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A391" s="1">
+        <v>45099</v>
+      </c>
+      <c r="B391">
+        <v>9410.8340000000007</v>
+      </c>
+      <c r="C391">
+        <v>9951.49</v>
+      </c>
+      <c r="D391">
+        <v>358.18</v>
+      </c>
+      <c r="E391">
+        <v>4045.29</v>
+      </c>
+      <c r="F391">
+        <v>138.41</v>
+      </c>
+      <c r="G391">
+        <v>102.5804</v>
+      </c>
+      <c r="H391">
+        <v>163.25</v>
+      </c>
+      <c r="I391">
+        <v>85.470500000000001</v>
+      </c>
+      <c r="J391">
+        <v>87.227099999999993</v>
+      </c>
+      <c r="K391">
+        <v>122.7086</v>
+      </c>
+      <c r="L391">
+        <v>870.34</v>
+      </c>
+      <c r="M391">
+        <v>1118.8399999999999</v>
+      </c>
+      <c r="N391">
+        <v>270.14659999999998</v>
+      </c>
+      <c r="O391">
+        <v>280.16000000000003</v>
+      </c>
+      <c r="P391">
+        <v>353.01</v>
+      </c>
+      <c r="Q391">
+        <v>336.68</v>
+      </c>
+      <c r="R391">
+        <v>168.14</v>
+      </c>
+    </row>
+    <row r="392" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A392" s="1">
+        <v>45100</v>
+      </c>
+      <c r="B392">
+        <v>9338.8349999999991</v>
+      </c>
+      <c r="C392">
+        <v>9875.5300000000007</v>
+      </c>
+      <c r="D392">
+        <v>354.78</v>
+      </c>
+      <c r="E392">
+        <v>4066.57</v>
+      </c>
+      <c r="F392">
+        <v>140.16999999999999</v>
+      </c>
+      <c r="G392">
+        <v>102.40260000000001</v>
+      </c>
+      <c r="H392">
+        <v>163.13999999999999</v>
+      </c>
+      <c r="I392">
+        <v>85.469800000000006</v>
+      </c>
+      <c r="J392">
+        <v>87.225300000000004</v>
+      </c>
+      <c r="K392">
+        <v>122.7077</v>
+      </c>
+      <c r="L392">
+        <v>870.99</v>
+      </c>
+      <c r="M392">
+        <v>1118.2</v>
+      </c>
+      <c r="N392">
+        <v>270.39909999999998</v>
+      </c>
+      <c r="O392">
+        <v>280.12</v>
+      </c>
+      <c r="P392">
+        <v>352.93</v>
+      </c>
+      <c r="Q392">
+        <v>336.57</v>
+      </c>
+      <c r="R392">
+        <v>168.21</v>
+      </c>
+    </row>
+    <row r="393" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A393" s="1">
+        <v>45103</v>
+      </c>
+      <c r="B393">
+        <v>9297.1229999999996</v>
+      </c>
+      <c r="C393">
+        <v>9896.23</v>
+      </c>
+      <c r="D393">
+        <v>353.88</v>
+      </c>
+      <c r="E393">
+        <v>4073.49</v>
+      </c>
+      <c r="F393">
+        <v>140.34</v>
+      </c>
+      <c r="G393">
+        <v>102.1653</v>
+      </c>
+      <c r="H393">
+        <v>162.99</v>
+      </c>
+      <c r="I393">
+        <v>85.468000000000004</v>
+      </c>
+      <c r="J393">
+        <v>87.223299999999995</v>
+      </c>
+      <c r="K393">
+        <v>122.7069</v>
+      </c>
+      <c r="L393">
+        <v>871.39</v>
+      </c>
+      <c r="M393">
+        <v>1118.93</v>
+      </c>
+      <c r="N393">
+        <v>270.61939999999998</v>
+      </c>
+      <c r="O393">
+        <v>280.13</v>
+      </c>
+      <c r="P393">
+        <v>353.07</v>
+      </c>
+      <c r="Q393">
+        <v>336.67</v>
+      </c>
+      <c r="R393">
+        <v>168.28</v>
+      </c>
+    </row>
+    <row r="394" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A394" s="1">
+        <v>45104</v>
+      </c>
+      <c r="B394">
+        <v>9403.6149999999998</v>
+      </c>
+      <c r="C394">
+        <v>9953.33</v>
+      </c>
+      <c r="D394">
+        <v>356.98</v>
+      </c>
+      <c r="E394">
+        <v>4065.44</v>
+      </c>
+      <c r="F394">
+        <v>139.97</v>
+      </c>
+      <c r="G394">
+        <v>102.2929</v>
+      </c>
+      <c r="H394">
+        <v>163.16999999999999</v>
+      </c>
+      <c r="I394">
+        <v>85.462000000000003</v>
+      </c>
+      <c r="J394">
+        <v>87.218400000000003</v>
+      </c>
+      <c r="K394">
+        <v>122.70359999999999</v>
+      </c>
+      <c r="L394">
+        <v>870.21</v>
+      </c>
+      <c r="M394">
+        <v>1116.8599999999999</v>
+      </c>
+      <c r="N394">
+        <v>270.32150000000001</v>
+      </c>
+      <c r="O394">
+        <v>279.70999999999998</v>
+      </c>
+      <c r="P394">
+        <v>352.44</v>
+      </c>
+      <c r="Q394">
+        <v>336.19</v>
+      </c>
+      <c r="R394">
+        <v>168.2</v>
+      </c>
+    </row>
+    <row r="395" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A395" s="1">
+        <v>45105</v>
+      </c>
+      <c r="B395">
+        <v>9400.3040000000001</v>
+      </c>
+      <c r="C395">
+        <v>10044.61</v>
+      </c>
+      <c r="D395">
+        <v>357.28</v>
+      </c>
+      <c r="E395">
+        <v>4084.78</v>
+      </c>
+      <c r="F395">
+        <v>140.66999999999999</v>
+      </c>
+      <c r="G395">
+        <v>101.98609999999999</v>
+      </c>
+      <c r="H395">
+        <v>163.03</v>
+      </c>
+      <c r="I395">
+        <v>85.460700000000003</v>
+      </c>
+      <c r="J395">
+        <v>87.215999999999994</v>
+      </c>
+      <c r="K395">
+        <v>122.703</v>
+      </c>
+      <c r="L395">
+        <v>870.26</v>
+      </c>
+      <c r="M395">
+        <v>1118.25</v>
+      </c>
+      <c r="N395">
+        <v>269.44589999999999</v>
+      </c>
+      <c r="O395">
+        <v>279.87</v>
+      </c>
+      <c r="P395">
+        <v>352.67</v>
+      </c>
+      <c r="Q395">
+        <v>336.32</v>
+      </c>
+      <c r="R395">
+        <v>168.38</v>
+      </c>
+    </row>
+    <row r="396" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A396" s="1">
+        <v>45106</v>
+      </c>
+      <c r="B396">
+        <v>9443.4650000000001</v>
+      </c>
+      <c r="C396">
+        <v>10067.61</v>
+      </c>
+      <c r="D396">
+        <v>358.15</v>
+      </c>
+      <c r="E396">
+        <v>4038.94</v>
+      </c>
+      <c r="F396">
+        <v>137.44999999999999</v>
+      </c>
+      <c r="G396">
+        <v>102.1409</v>
+      </c>
+      <c r="H396">
+        <v>163.15</v>
+      </c>
+      <c r="I396">
+        <v>85.460400000000007</v>
+      </c>
+      <c r="J396">
+        <v>87.215999999999994</v>
+      </c>
+      <c r="K396">
+        <v>122.703</v>
+      </c>
+      <c r="L396">
+        <v>869.83</v>
+      </c>
+      <c r="M396">
+        <v>1116.82</v>
+      </c>
+      <c r="N396">
+        <v>268.6121</v>
+      </c>
+      <c r="O396">
+        <v>279.89</v>
+      </c>
+      <c r="P396">
+        <v>352.69</v>
+      </c>
+      <c r="Q396">
+        <v>336.2</v>
+      </c>
+      <c r="R396">
+        <v>168.2</v>
+      </c>
+    </row>
+    <row r="397" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A397" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B397">
+        <v>9559.6659999999993</v>
+      </c>
+      <c r="C397">
+        <v>10170.26</v>
+      </c>
+      <c r="D397">
+        <v>361.86</v>
+      </c>
+      <c r="E397">
+        <v>4082.76</v>
+      </c>
+      <c r="F397">
+        <v>139.72999999999999</v>
+      </c>
+      <c r="G397">
+        <v>102.498</v>
+      </c>
+      <c r="H397">
+        <v>163.22999999999999</v>
+      </c>
+      <c r="I397">
+        <v>85.456800000000001</v>
+      </c>
+      <c r="J397">
+        <v>87.212900000000005</v>
+      </c>
+      <c r="K397">
+        <v>122.70099999999999</v>
+      </c>
+      <c r="L397">
+        <v>868.82</v>
+      </c>
+      <c r="M397">
+        <v>1112.27</v>
+      </c>
+      <c r="N397">
+        <v>269.27850000000001</v>
+      </c>
+      <c r="O397">
+        <v>279.79000000000002</v>
+      </c>
+      <c r="P397">
+        <v>352.56</v>
+      </c>
+      <c r="Q397">
+        <v>336.05</v>
+      </c>
+      <c r="R397">
+        <v>167.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove benchmarks from equity hedge data
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_data/ups_data.xlsx
+++ b/EquityHedging/data/update_data/ups_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\RMP\EquityHedging\data\update_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14053A54-B2AE-42BC-916E-8D240FDDD790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BE802C-5E7B-4036-8566-9F9D23B81F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28910" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28910" yWindow="0" windowWidth="29020" windowHeight="15820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="24">
   <si>
     <t>SPTR Index</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>End Date</t>
-  </si>
-  <si>
-    <t>I20659US Index</t>
   </si>
   <si>
     <t>CSEADP2E Index</t>
@@ -184,102 +181,72 @@
   <volType type="realTimeData">
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...3926466388</v>
+        <v>#N/A Requesting Data...3747310377</v>
         <stp/>
-        <stp>BDH|12446595102625011047</stp>
-        <tr r="E7" s="4"/>
+        <stp>BDH|12214759940403984135</stp>
+        <tr r="M7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4014557279</v>
+        <v>#N/A Requesting Data...2798922603</v>
         <stp/>
-        <stp>BDH|12214759940403984135</stp>
-        <tr r="R7" s="4"/>
+        <stp>BDH|16332318276436657497</stp>
+        <tr r="G7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3516932590</v>
-        <stp/>
-        <stp>BDH|16332318276436657497</stp>
-        <tr r="L7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...3792883865</v>
+        <v>#N/A Requesting Data...3066251401</v>
         <stp/>
         <stp>BDH|12478626226644177700</stp>
-        <tr r="K7" s="4"/>
+        <tr r="F7" s="4"/>
       </tp>
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...4220003301</v>
+        <v>#N/A Requesting Data...4101844923</v>
         <stp/>
         <stp>BDH|5676996075887292050</stp>
-        <tr r="G7" s="4"/>
+        <tr r="B7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3769759073</v>
+        <v>#N/A Requesting Data...2660700559</v>
         <stp/>
-        <stp>BDH|5194611918228677719</stp>
-        <tr r="F7" s="4"/>
+        <stp>BDH|4340614083227769361</stp>
+        <tr r="K7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3880793078</v>
+        <v>#N/A Requesting Data...2299153986</v>
         <stp/>
-        <stp>BDH|4340614083227769361</stp>
-        <tr r="P7" s="4"/>
+        <stp>BDH|4466424671208990742</stp>
+        <tr r="L7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3740340682</v>
-        <stp/>
-        <stp>BDH|8918062699976416876</stp>
-        <tr r="A7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...3648359903</v>
-        <stp/>
-        <stp>BDH|4466424671208990742</stp>
-        <tr r="Q7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4149591944</v>
+        <v>#N/A Requesting Data...3464085171</v>
         <stp/>
         <stp>BDH|2573669918646284975</stp>
-        <tr r="N7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...3600969440</v>
-        <stp/>
-        <stp>BDH|5731873043626887426</stp>
         <tr r="I7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...3673449572</v>
+        <v>#N/A Requesting Data...2469734233</v>
+        <stp/>
+        <stp>BDH|5731873043626887426</stp>
+        <tr r="D7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...2883108239</v>
         <stp/>
         <stp>BDH|9948447770906973749</stp>
+        <tr r="C7" s="4"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A Requesting Data...4043346415</v>
+        <stp/>
+        <stp>BDH|2427336485935611957</stp>
         <tr r="H7" s="4"/>
       </tp>
       <tp t="s">
-        <v>#N/A Requesting Data...4149837620</v>
-        <stp/>
-        <stp>BDH|6444104926092977241</stp>
-        <tr r="D7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4109796563</v>
-        <stp/>
-        <stp>BDH|2427336485935611957</stp>
-        <tr r="M7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...4215503514</v>
+        <v>#N/A Requesting Data...2887550827</v>
         <stp/>
         <stp>BDH|3616900091481663403</stp>
-        <tr r="J7" s="4"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A Requesting Data...3923634206</v>
-        <stp/>
-        <stp>BDH|8790272014849135324</stp>
-        <tr r="C7" s="4"/>
+        <tr r="E7" s="4"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -314,46 +281,6 @@
         <stp>[ups_data.xlsx]bbg!R5C10</stp>
         <stp>PX_LAST</stp>
         <tr r="J5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C17</stp>
-        <stp>PX_LAST</stp>
-        <tr r="Q5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C16</stp>
-        <stp>PX_LAST</stp>
-        <tr r="P5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C15</stp>
-        <stp>PX_LAST</stp>
-        <tr r="O5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C14</stp>
-        <stp>PX_LAST</stp>
-        <tr r="N5" s="4"/>
-      </tp>
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>##V3_BFIELDINFOV12</stp>
-        <stp>[ups_data.xlsx]bbg!R5C18</stp>
-        <stp>PX_LAST</stp>
-        <tr r="R5" s="4"/>
       </tp>
       <tp t="e">
         <v>#N/A</v>
@@ -422,10 +349,10 @@
     </main>
     <main first="bofaddin.rtdserver">
       <tp t="s">
-        <v>#N/A Requesting Data...4254863650</v>
+        <v>#N/A Requesting Data...4037681193</v>
         <stp/>
         <stp>BDH|850395225739575272</stp>
-        <tr r="O7" s="4"/>
+        <tr r="J7" s="4"/>
       </tp>
     </main>
   </volType>
@@ -697,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M807"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -734,7 +661,7 @@
         <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -752,7 +679,7 @@
         <v>14</v>
       </c>
       <c r="M1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -775,7 +702,7 @@
         <v>155.67609999999999</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2">
         <v>1109.05</v>
@@ -33827,10 +33754,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -33841,10 +33768,10 @@
         <v>2306.232</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -33855,10 +33782,10 @@
         <v>2306.232</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -33869,10 +33796,10 @@
         <v>2273.4059999999999</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -33883,10 +33810,10 @@
         <v>2273.4140000000002</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -33897,10 +33824,10 @@
         <v>2217.5920000000001</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -33911,10 +33838,10 @@
         <v>2224.761</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -33925,10 +33852,10 @@
         <v>2184.6669999999999</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -33939,10 +33866,10 @@
         <v>2214.6019999999999</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -33953,10 +33880,10 @@
         <v>2232.2449999999999</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -33967,10 +33894,10 @@
         <v>2202.027</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -33981,10 +33908,10 @@
         <v>2225.9760000000001</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -33995,10 +33922,10 @@
         <v>2170.5100000000002</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -34009,10 +33936,10 @@
         <v>2158.5749999999998</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -34023,10 +33950,10 @@
         <v>2095.8609999999999</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -84380,10 +84307,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R812"/>
+  <dimension ref="A1:M812"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -84406,7 +84333,7 @@
     <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -84414,7 +84341,7 @@
         <v>43980</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -84422,60 +84349,45 @@
         <v>45107</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
       <c r="H4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M4" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" t="s">
-        <v>9</v>
-      </c>
-      <c r="O4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>14</v>
-      </c>
-      <c r="R4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B5" t="e">
         <f>_xll.BFieldInfo(B$6)</f>
         <v>#N/A</v>
@@ -84524,86 +84436,55 @@
         <f>_xll.BFieldInfo(M$6)</f>
         <v>#N/A</v>
       </c>
-      <c r="N5" t="e">
-        <f>_xll.BFieldInfo(N$6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O5" t="e">
-        <f>_xll.BFieldInfo(O$6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P5" t="e">
-        <f>_xll.BFieldInfo(P$6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q5" t="e">
-        <f>_xll.BFieldInfo(Q$6)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R5" t="e">
-        <f>_xll.BFieldInfo(R$6)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="str">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S")</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="e">
+        <f>_xll.BDH(#REF!,#REF!,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=S")</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B7" t="str">
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H")</f>
         <v>#N/A Connection</v>
       </c>
       <c r="C7" t="str">
@@ -84650,52 +84531,32 @@
         <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H")</f>
         <v>#N/A Connection</v>
       </c>
-      <c r="N7" t="str">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H")</f>
-        <v>#N/A Connection</v>
-      </c>
-      <c r="O7" t="str">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H")</f>
-        <v>#N/A Connection</v>
-      </c>
-      <c r="P7" t="str">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H")</f>
-        <v>#N/A Connection</v>
-      </c>
-      <c r="Q7" t="str">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H")</f>
-        <v>#N/A Connection</v>
-      </c>
-      <c r="R7" t="str">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","CDR=5D","Days=A","Dts=H")</f>
-        <v>#N/A Connection</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
@@ -87152,7 +87013,7 @@
         <v>15</v>
       </c>
       <c r="L1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>

</xml_diff>